<commit_message>
Renamed Process Flow Diagram. Added some more BOM items.
</commit_message>
<xml_diff>
--- a/V1 BOM.xlsx
+++ b/V1 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f1d977de6d9a3fe/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\apfc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="723" documentId="8_{449518B1-EDD0-4B52-8A59-8200D3DE19AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FA2E5CA-38BE-4F2E-A164-901C3524DDFD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E77A62-F498-4684-A5CD-2B35DE53320E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3795" yWindow="3105" windowWidth="23265" windowHeight="12195" xr2:uid="{90341DFA-DDFA-4A7D-AB9C-A22698E387D2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="199">
   <si>
     <t>HPA Irrigation Pump</t>
   </si>
@@ -613,6 +613,27 @@
   </si>
   <si>
     <t>DG257</t>
+  </si>
+  <si>
+    <t>Stop cap for waste water valve</t>
+  </si>
+  <si>
+    <t>Brass Blanking Caps 1/2" (Pack of 3) with Washers for 15mm Compression Fittings</t>
+  </si>
+  <si>
+    <t>‎LP Supplies</t>
+  </si>
+  <si>
+    <t>TDS sensors for filter change checking</t>
+  </si>
+  <si>
+    <t>CQRobot Ocean: TDS (Total Dissolved Solids) Meter Sensor Compatible with Raspberry Pi/Arduino Board. for Liquid Quality Analysis Teaching, Scientific Research, Laboratory, Online Analysis, etc.</t>
+  </si>
+  <si>
+    <t>CQRobot</t>
+  </si>
+  <si>
+    <t>CQRSENTDS01</t>
   </si>
 </sst>
 </file>
@@ -706,10 +727,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1009,12 +1026,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F40200-5B19-4188-8D38-5918C89D4CBF}">
-  <dimension ref="B1:K46"/>
+  <dimension ref="B1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1105,7 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2">
-        <f>G2*J2</f>
+        <f t="shared" ref="K2:K48" si="0">G2*J2</f>
         <v>0</v>
       </c>
     </row>
@@ -1115,14 +1132,14 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I46" si="0">G3*H3</f>
+        <f t="shared" ref="I3:I48" si="1">G3*H3</f>
         <v>1</v>
       </c>
       <c r="J3" s="2">
         <v>5.99</v>
       </c>
       <c r="K3" s="2">
-        <f>G3*J3</f>
+        <f t="shared" si="0"/>
         <v>5.99</v>
       </c>
     </row>
@@ -1146,14 +1163,14 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J4" s="2">
         <v>7.49</v>
       </c>
       <c r="K4" s="2">
-        <f>G4*J4</f>
+        <f t="shared" si="0"/>
         <v>7.49</v>
       </c>
     </row>
@@ -1177,14 +1194,14 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J5" s="2">
         <v>48.99</v>
       </c>
       <c r="K5" s="2">
-        <f>G5*J5</f>
+        <f t="shared" si="0"/>
         <v>48.99</v>
       </c>
     </row>
@@ -1211,14 +1228,14 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J6" s="2">
         <v>54.84</v>
       </c>
       <c r="K6" s="2">
-        <f>G6*J6</f>
+        <f t="shared" si="0"/>
         <v>54.84</v>
       </c>
     </row>
@@ -1242,14 +1259,14 @@
         <v>20</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J7" s="2">
         <v>11.99</v>
       </c>
       <c r="K7" s="2">
-        <f>G7*J7</f>
+        <f t="shared" si="0"/>
         <v>11.99</v>
       </c>
     </row>
@@ -1276,14 +1293,14 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J8" s="2">
         <v>8.99</v>
       </c>
       <c r="K8" s="2">
-        <f>G8*J8</f>
+        <f t="shared" si="0"/>
         <v>8.99</v>
       </c>
     </row>
@@ -1310,14 +1327,14 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J9" s="2">
         <v>16.29</v>
       </c>
       <c r="K9" s="2">
-        <f>G9*J9</f>
+        <f t="shared" si="0"/>
         <v>16.29</v>
       </c>
     </row>
@@ -1344,14 +1361,14 @@
         <v>5</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J10" s="2">
         <v>8.49</v>
       </c>
       <c r="K10" s="2">
-        <f>G10*J10</f>
+        <f t="shared" si="0"/>
         <v>8.49</v>
       </c>
     </row>
@@ -1378,14 +1395,14 @@
         <v>2</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J11" s="2">
         <v>8.49</v>
       </c>
       <c r="K11" s="2">
-        <f>G11*J11</f>
+        <f t="shared" si="0"/>
         <v>8.49</v>
       </c>
     </row>
@@ -1412,14 +1429,14 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J12" s="2">
         <v>7.98</v>
       </c>
       <c r="K12" s="2">
-        <f>G12*J12</f>
+        <f t="shared" si="0"/>
         <v>7.98</v>
       </c>
     </row>
@@ -1446,14 +1463,14 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J13" s="2">
         <v>14.99</v>
       </c>
       <c r="K13" s="2">
-        <f>G13*J13</f>
+        <f t="shared" si="0"/>
         <v>14.99</v>
       </c>
     </row>
@@ -1477,14 +1494,14 @@
         <v>3</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J14" s="2">
         <v>8.09</v>
       </c>
       <c r="K14" s="2">
-        <f>G14*J14</f>
+        <f t="shared" si="0"/>
         <v>8.09</v>
       </c>
     </row>
@@ -1508,14 +1525,14 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="J15" s="2">
         <v>6.24</v>
       </c>
       <c r="K15" s="2">
-        <f>G15*J15</f>
+        <f t="shared" si="0"/>
         <v>37.44</v>
       </c>
     </row>
@@ -1539,14 +1556,14 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J16" s="2">
         <v>8.99</v>
       </c>
       <c r="K16" s="2">
-        <f>G16*J16</f>
+        <f t="shared" si="0"/>
         <v>8.99</v>
       </c>
     </row>
@@ -1570,14 +1587,14 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J17" s="2">
         <v>9.59</v>
       </c>
       <c r="K17" s="2">
-        <f>G17*J17</f>
+        <f t="shared" si="0"/>
         <v>9.59</v>
       </c>
     </row>
@@ -1601,14 +1618,14 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J18" s="2">
         <v>17.989999999999998</v>
       </c>
       <c r="K18" s="2">
-        <f>G18*J18</f>
+        <f t="shared" si="0"/>
         <v>35.979999999999997</v>
       </c>
     </row>
@@ -1635,14 +1652,14 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J19" s="2">
         <v>6.59</v>
       </c>
       <c r="K19" s="2">
-        <f>G19*J19</f>
+        <f t="shared" si="0"/>
         <v>19.77</v>
       </c>
     </row>
@@ -1666,14 +1683,14 @@
         <v>12</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="J20" s="2">
         <v>7.99</v>
       </c>
       <c r="K20" s="2">
-        <f>G20*J20</f>
+        <f t="shared" si="0"/>
         <v>15.98</v>
       </c>
     </row>
@@ -1697,14 +1714,14 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J21" s="2">
         <v>7.99</v>
       </c>
       <c r="K21" s="2">
-        <f>G21*J21</f>
+        <f t="shared" si="0"/>
         <v>7.99</v>
       </c>
     </row>
@@ -1728,14 +1745,14 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J22" s="2">
         <v>9.49</v>
       </c>
       <c r="K22" s="2">
-        <f>G22*J22</f>
+        <f t="shared" si="0"/>
         <v>37.96</v>
       </c>
     </row>
@@ -1759,14 +1776,14 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J23" s="2">
         <v>8.1</v>
       </c>
       <c r="K23" s="2">
-        <f>G23*J23</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
     </row>
@@ -1790,14 +1807,14 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J24" s="2">
         <v>10.99</v>
       </c>
       <c r="K24" s="2">
-        <f>G24*J24</f>
+        <f t="shared" si="0"/>
         <v>32.97</v>
       </c>
     </row>
@@ -1824,14 +1841,14 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J25" s="2">
         <v>6</v>
       </c>
       <c r="K25" s="2">
-        <f>G25*J25</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -1858,14 +1875,14 @@
         <v>1</v>
       </c>
       <c r="I26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J26" s="2">
         <v>13.5</v>
       </c>
       <c r="K26" s="2">
-        <f>G26*J26</f>
+        <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
     </row>
@@ -1892,14 +1909,14 @@
         <v>1</v>
       </c>
       <c r="I27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J27" s="2">
         <v>4.49</v>
       </c>
       <c r="K27" s="2">
-        <f>G27*J27</f>
+        <f t="shared" si="0"/>
         <v>4.49</v>
       </c>
     </row>
@@ -1926,14 +1943,14 @@
         <v>1</v>
       </c>
       <c r="I28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J28" s="2">
         <v>4.29</v>
       </c>
       <c r="K28" s="2">
-        <f>G28*J28</f>
+        <f t="shared" si="0"/>
         <v>4.29</v>
       </c>
     </row>
@@ -1960,14 +1977,14 @@
         <v>1</v>
       </c>
       <c r="I29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J29" s="2">
         <v>1.89</v>
       </c>
       <c r="K29" s="2">
-        <f>G29*J29</f>
+        <f t="shared" si="0"/>
         <v>1.89</v>
       </c>
     </row>
@@ -1994,14 +2011,14 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J30" s="2">
         <v>1.99</v>
       </c>
       <c r="K30" s="2">
-        <f>G30*J30</f>
+        <f t="shared" si="0"/>
         <v>3.98</v>
       </c>
     </row>
@@ -2028,14 +2045,14 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J31" s="2">
         <v>6.49</v>
       </c>
       <c r="K31" s="2">
-        <f>G31*J31</f>
+        <f t="shared" si="0"/>
         <v>6.49</v>
       </c>
     </row>
@@ -2059,14 +2076,14 @@
         <v>1</v>
       </c>
       <c r="I32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J32" s="2">
         <v>8.8699999999999992</v>
       </c>
       <c r="K32" s="2">
-        <f>G32*J32</f>
+        <f t="shared" si="0"/>
         <v>17.739999999999998</v>
       </c>
     </row>
@@ -2093,14 +2110,14 @@
         <v>8</v>
       </c>
       <c r="I33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="J33" s="2">
         <v>7.49</v>
       </c>
       <c r="K33" s="2">
-        <f>G33*J33</f>
+        <f t="shared" si="0"/>
         <v>14.98</v>
       </c>
     </row>
@@ -2127,14 +2144,14 @@
         <v>1</v>
       </c>
       <c r="I34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J34" s="2">
         <v>30</v>
       </c>
       <c r="K34" s="2">
-        <f>G34*J34</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -2161,14 +2178,14 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J35" s="2">
         <v>53.9</v>
       </c>
       <c r="K35" s="2">
-        <f>G35*J35</f>
+        <f t="shared" si="0"/>
         <v>53.9</v>
       </c>
     </row>
@@ -2195,14 +2212,14 @@
         <v>1</v>
       </c>
       <c r="I36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J36" s="2">
         <v>17.05</v>
       </c>
       <c r="K36" s="2">
-        <f>G36*J36</f>
+        <f t="shared" si="0"/>
         <v>17.05</v>
       </c>
     </row>
@@ -2229,14 +2246,14 @@
         <v>1</v>
       </c>
       <c r="I37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J37" s="2">
         <v>5.18</v>
       </c>
       <c r="K37" s="2">
-        <f>G37*J37</f>
+        <f t="shared" si="0"/>
         <v>5.18</v>
       </c>
     </row>
@@ -2263,14 +2280,14 @@
         <v>1</v>
       </c>
       <c r="I38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J38" s="2">
         <v>14.9</v>
       </c>
       <c r="K38" s="2">
-        <f>G38*J38</f>
+        <f t="shared" si="0"/>
         <v>29.8</v>
       </c>
     </row>
@@ -2297,14 +2314,14 @@
         <v>1</v>
       </c>
       <c r="I39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J39" s="2">
         <v>139.99</v>
       </c>
       <c r="K39" s="2">
-        <f>G39*J39</f>
+        <f t="shared" si="0"/>
         <v>139.99</v>
       </c>
     </row>
@@ -2331,14 +2348,14 @@
         <v>1</v>
       </c>
       <c r="I40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J40" s="2">
         <v>27.99</v>
       </c>
       <c r="K40" s="2">
-        <f>G40*J40</f>
+        <f t="shared" si="0"/>
         <v>27.99</v>
       </c>
     </row>
@@ -2365,14 +2382,14 @@
         <v>1</v>
       </c>
       <c r="I41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J41" s="2">
         <v>57.6</v>
       </c>
       <c r="K41" s="2">
-        <f>G41*J41</f>
+        <f t="shared" si="0"/>
         <v>115.2</v>
       </c>
     </row>
@@ -2399,14 +2416,14 @@
         <v>12</v>
       </c>
       <c r="I42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="J42" s="2">
         <v>6.34</v>
       </c>
       <c r="K42" s="2">
-        <f>G42*J42</f>
+        <f t="shared" si="0"/>
         <v>6.34</v>
       </c>
     </row>
@@ -2433,14 +2450,14 @@
         <v>10</v>
       </c>
       <c r="I43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J43" s="2">
         <v>32.1</v>
       </c>
       <c r="K43" s="2">
-        <f>G43*J43</f>
+        <f t="shared" si="0"/>
         <v>32.1</v>
       </c>
     </row>
@@ -2467,14 +2484,14 @@
         <v>2</v>
       </c>
       <c r="I44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J44" s="2">
         <v>19.98</v>
       </c>
       <c r="K44" s="2">
-        <f>G44*J44</f>
+        <f t="shared" si="0"/>
         <v>79.92</v>
       </c>
     </row>
@@ -2498,14 +2515,14 @@
         <v>1</v>
       </c>
       <c r="I45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J45" s="2">
         <v>18.47</v>
       </c>
       <c r="K45" s="2">
-        <f>G45*J45</f>
+        <f t="shared" si="0"/>
         <v>18.47</v>
       </c>
     </row>
@@ -2532,15 +2549,83 @@
         <v>2</v>
       </c>
       <c r="I46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J46" s="2">
         <v>8.99</v>
       </c>
       <c r="K46" s="2">
-        <f>G46*J46</f>
+        <f t="shared" si="0"/>
         <v>8.99</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>192</v>
+      </c>
+      <c r="C47" t="s">
+        <v>194</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E47">
+        <v>10070227</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J47" s="2">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="K47" s="2">
+        <f t="shared" si="0"/>
+        <v>4.3899999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>195</v>
+      </c>
+      <c r="C48" t="s">
+        <v>197</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E48" t="s">
+        <v>198</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J48" s="2">
+        <v>10.99</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="0"/>
+        <v>21.98</v>
       </c>
     </row>
   </sheetData>
@@ -2589,9 +2674,11 @@
     <hyperlink ref="F44" r:id="rId42" xr:uid="{FBD0A3BF-4175-4C32-BD62-0DB032380A67}"/>
     <hyperlink ref="F45" r:id="rId43" xr:uid="{F6A85D1A-D25E-4DF2-9558-E9CEDA803A57}"/>
     <hyperlink ref="F46" r:id="rId44" xr:uid="{B6CE8CFB-D10B-4506-936C-F2E913C84081}"/>
+    <hyperlink ref="F47" r:id="rId45" xr:uid="{1B5536CF-3ABF-4E7F-AF15-C6D12C94C388}"/>
+    <hyperlink ref="F48" r:id="rId46" xr:uid="{157391B4-665F-417E-8BF8-96E41D45FE97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Laser cutting templates and 3D printing GCode
</commit_message>
<xml_diff>
--- a/V1 BOM.xlsx
+++ b/V1 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\apfc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E77A62-F498-4684-A5CD-2B35DE53320E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A728FA-05E1-4123-BF84-88A9897BBD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3795" yWindow="3105" windowWidth="23265" windowHeight="12195" xr2:uid="{90341DFA-DDFA-4A7D-AB9C-A22698E387D2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="205">
   <si>
     <t>HPA Irrigation Pump</t>
   </si>
@@ -634,6 +634,24 @@
   </si>
   <si>
     <t>CQRSENTDS01</t>
+  </si>
+  <si>
+    <t>Waste water tap</t>
+  </si>
+  <si>
+    <t>RMTL</t>
+  </si>
+  <si>
+    <t>RMTL Outdoor Garden Tap Hose Union Bib Tap 1/2inch BSP with Compression Wallplate Elbow, Through The Wall 15mm Copper Tube (Single Bib Tap)</t>
+  </si>
+  <si>
+    <t>Sourcingmap 50 Pcs M2 x 15mm Stainless Steel Phillips Round Head Self Tapping Screws Bolts</t>
+  </si>
+  <si>
+    <t>a16072200ux0833</t>
+  </si>
+  <si>
+    <t>Plumbing bracket mounting screws</t>
   </si>
 </sst>
 </file>
@@ -1026,12 +1044,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F40200-5B19-4188-8D38-5918C89D4CBF}">
-  <dimension ref="B1:K48"/>
+  <dimension ref="B1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,7 +1123,7 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2">
-        <f t="shared" ref="K2:K48" si="0">G2*J2</f>
+        <f t="shared" ref="K2:K50" si="0">G2*J2</f>
         <v>0</v>
       </c>
     </row>
@@ -1132,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I48" si="1">G3*H3</f>
+        <f t="shared" ref="I3:I50" si="1">G3*H3</f>
         <v>1</v>
       </c>
       <c r="J3" s="2">
@@ -2626,6 +2644,71 @@
       <c r="K48" s="2">
         <f t="shared" si="0"/>
         <v>21.98</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" t="s">
+        <v>200</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J49" s="2">
+        <v>8.99</v>
+      </c>
+      <c r="K49" s="2">
+        <f t="shared" si="0"/>
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>204</v>
+      </c>
+      <c r="C50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E50" t="s">
+        <v>203</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>50</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J50" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="K50" s="2">
+        <f t="shared" si="0"/>
+        <v>5.99</v>
       </c>
     </row>
   </sheetData>
@@ -2676,9 +2759,11 @@
     <hyperlink ref="F46" r:id="rId44" xr:uid="{B6CE8CFB-D10B-4506-936C-F2E913C84081}"/>
     <hyperlink ref="F47" r:id="rId45" xr:uid="{1B5536CF-3ABF-4E7F-AF15-C6D12C94C388}"/>
     <hyperlink ref="F48" r:id="rId46" xr:uid="{157391B4-665F-417E-8BF8-96E41D45FE97}"/>
+    <hyperlink ref="F49" r:id="rId47" xr:uid="{66446346-8333-4F64-BB83-350FFBC22F5A}"/>
+    <hyperlink ref="F50" r:id="rId48" xr:uid="{5BF9A1AF-7F88-4282-8F74-420CFBE5A5DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Picked out components for nutrient management
</commit_message>
<xml_diff>
--- a/V1 BOM.xlsx
+++ b/V1 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\apfc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A728FA-05E1-4123-BF84-88A9897BBD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD21191-E5B6-4F2B-BB2C-89076E436A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3795" yWindow="3105" windowWidth="23265" windowHeight="12195" xr2:uid="{90341DFA-DDFA-4A7D-AB9C-A22698E387D2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="213">
   <si>
     <t>HPA Irrigation Pump</t>
   </si>
@@ -652,6 +652,30 @@
   </si>
   <si>
     <t>Plumbing bracket mounting screws</t>
+  </si>
+  <si>
+    <t>Water temperature sensor</t>
+  </si>
+  <si>
+    <t>Aideepen</t>
+  </si>
+  <si>
+    <t>Aideepen 5 x DS18B20 2m Cable Temperature Digital Thermal Probe Sensor Stainless Steel Probe, Accurate Reading, Measure Temperature -55°C to +125°C</t>
+  </si>
+  <si>
+    <t>A70110795UK</t>
+  </si>
+  <si>
+    <t>Nutrient solution heater</t>
+  </si>
+  <si>
+    <t>Hidom</t>
+  </si>
+  <si>
+    <t>‎HT-2025-U</t>
+  </si>
+  <si>
+    <t>Hidom 25w Submersible Aquarium Fish Tank Shockproof Thermostat Heater - Adjustable Temperature HT-2025</t>
   </si>
 </sst>
 </file>
@@ -1044,12 +1068,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F40200-5B19-4188-8D38-5918C89D4CBF}">
-  <dimension ref="B1:K50"/>
+  <dimension ref="B1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
+      <selection pane="bottomLeft" activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1147,7 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2">
-        <f t="shared" ref="K2:K50" si="0">G2*J2</f>
+        <f t="shared" ref="K2:K52" si="0">G2*J2</f>
         <v>0</v>
       </c>
     </row>
@@ -1150,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I50" si="1">G3*H3</f>
+        <f t="shared" ref="I3:I52" si="1">G3*H3</f>
         <v>1</v>
       </c>
       <c r="J3" s="2">
@@ -2709,6 +2733,74 @@
       <c r="K50" s="2">
         <f t="shared" si="0"/>
         <v>5.99</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>205</v>
+      </c>
+      <c r="C51" t="s">
+        <v>206</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E51" t="s">
+        <v>208</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J51" s="2">
+        <v>11.99</v>
+      </c>
+      <c r="K51" s="2">
+        <f t="shared" si="0"/>
+        <v>11.99</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>209</v>
+      </c>
+      <c r="C52" t="s">
+        <v>210</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E52" t="s">
+        <v>211</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J52" s="2">
+        <v>10.45</v>
+      </c>
+      <c r="K52" s="2">
+        <f t="shared" si="0"/>
+        <v>10.45</v>
       </c>
     </row>
   </sheetData>
@@ -2761,9 +2853,11 @@
     <hyperlink ref="F48" r:id="rId46" xr:uid="{157391B4-665F-417E-8BF8-96E41D45FE97}"/>
     <hyperlink ref="F49" r:id="rId47" xr:uid="{66446346-8333-4F64-BB83-350FFBC22F5A}"/>
     <hyperlink ref="F50" r:id="rId48" xr:uid="{5BF9A1AF-7F88-4282-8F74-420CFBE5A5DE}"/>
+    <hyperlink ref="F51" r:id="rId49" xr:uid="{E20B2BE7-5BA7-47EA-AA81-840AA8C848AA}"/>
+    <hyperlink ref="F52" r:id="rId50" xr:uid="{E4B57222-4F24-4E9D-957D-1BEE53DE8072}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId49"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 

</xml_diff>